<commit_message>
latest update and upgrade to laravel 7.0
</commit_message>
<xml_diff>
--- a/public/fileku/guruxls.xlsx
+++ b/public/fileku/guruxls.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\difka\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\difka\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -125,10 +125,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -413,17 +414,17 @@
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="19.42578125" customWidth="1"/>
     <col min="3" max="3" width="21.7109375" customWidth="1"/>
-    <col min="4" max="4" width="17.5703125" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" style="3" customWidth="1"/>
     <col min="6" max="6" width="16.85546875" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="22.42578125" customWidth="1"/>
     <col min="9" max="9" width="32.7109375" customWidth="1"/>
     <col min="10" max="10" width="26.140625" customWidth="1"/>
@@ -472,7 +473,7 @@
       <c r="C2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="3">
         <v>98122</v>
       </c>
       <c r="F2">
@@ -498,7 +499,7 @@
       <c r="C3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="3">
         <v>921821</v>
       </c>
       <c r="F3">

</xml_diff>